<commit_message>
Added new sheet METEO
</commit_message>
<xml_diff>
--- a/resources/model_variables_mask.xlsx
+++ b/resources/model_variables_mask.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikel\Documents\VICOMTECH\Info y datos EDAR Cartuja\0.0-Definicion Caso de Uso 01_AManas-ERoche\Datos\08.01-Enviado_a_DVelasquez_VIC_2019-11-18_V1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvelasquez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8140B6-3318-49E8-88F1-05BCA4EB1E84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="989" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6945" tabRatio="989" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ID_INFLUENTE" sheetId="1" r:id="rId1"/>
@@ -21,8 +20,9 @@
     <sheet name="ID_ELECTRICIDAD" sheetId="6" r:id="rId6"/>
     <sheet name="YOKO" sheetId="7" r:id="rId7"/>
     <sheet name="ANALITICA" sheetId="8" r:id="rId8"/>
+    <sheet name="METEO" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191028" iterate="1"/>
+  <calcPr calcId="152511" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="251">
   <si>
     <t>ORIGEN</t>
   </si>
@@ -767,13 +767,34 @@
   </si>
   <si>
     <t>ANALITICA</t>
+  </si>
+  <si>
+    <t>P24</t>
+  </si>
+  <si>
+    <t>TMED</t>
+  </si>
+  <si>
+    <t>PRES00</t>
+  </si>
+  <si>
+    <t>PRES07</t>
+  </si>
+  <si>
+    <t>PRES13</t>
+  </si>
+  <si>
+    <t>PRES18</t>
+  </si>
+  <si>
+    <t>METEO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -789,6 +810,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -845,7 +872,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -863,6 +890,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1176,26 +1204,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" customWidth="1"/>
-    <col min="8" max="1025" width="10.7265625"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1246,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1232,7 +1260,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1246,7 +1274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1260,7 +1288,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1271,7 +1299,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1282,7 +1310,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1293,7 +1321,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1304,7 +1332,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1315,7 +1343,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1326,7 +1354,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1337,7 +1365,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1348,7 +1376,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1359,7 +1387,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1370,7 +1398,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1381,7 +1409,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1392,7 +1420,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1403,7 +1431,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1414,7 +1442,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1425,7 +1453,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1436,12 +1464,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E21" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E22" s="6" t="s">
         <v>13</v>
       </c>
@@ -1453,26 +1481,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="1025" width="13.453125"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="13.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1495,7 +1523,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1518,7 +1546,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1537,8 +1565,11 @@
       <c r="F3" s="9" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1558,7 +1589,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -1575,7 +1606,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -1592,7 +1623,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1609,7 +1640,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -1626,7 +1657,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1643,7 +1674,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -1660,7 +1691,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -1677,7 +1708,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -1691,7 +1722,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -1705,7 +1736,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>95</v>
       </c>
@@ -1719,7 +1750,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -1733,7 +1764,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -1744,7 +1775,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -1755,7 +1786,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>105</v>
       </c>
@@ -1763,7 +1794,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>106</v>
       </c>
@@ -1771,7 +1802,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>107</v>
       </c>
@@ -1779,7 +1810,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -1787,7 +1818,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -1795,7 +1826,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -1803,7 +1834,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -1811,7 +1842,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -1819,7 +1850,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>113</v>
       </c>
@@ -1827,7 +1858,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -1835,7 +1866,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>115</v>
       </c>
@@ -1843,7 +1874,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>116</v>
       </c>
@@ -1851,7 +1882,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>117</v>
       </c>
@@ -1859,7 +1890,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>118</v>
       </c>
@@ -1867,7 +1898,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -1875,7 +1906,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>120</v>
       </c>
@@ -1883,7 +1914,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>121</v>
       </c>
@@ -1891,7 +1922,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>122</v>
       </c>
@@ -1899,7 +1930,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>123</v>
       </c>
@@ -1907,7 +1938,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>124</v>
       </c>
@@ -1915,7 +1946,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>125</v>
       </c>
@@ -1923,7 +1954,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>126</v>
       </c>
@@ -1931,7 +1962,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>127</v>
       </c>
@@ -1939,7 +1970,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>128</v>
       </c>
@@ -1947,7 +1978,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>129</v>
       </c>
@@ -1962,24 +1993,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2002,7 +2033,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2022,7 +2053,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -2045,7 +2076,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>133</v>
       </c>
@@ -2065,7 +2096,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>135</v>
       </c>
@@ -2085,7 +2116,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>137</v>
       </c>
@@ -2101,8 +2132,11 @@
       <c r="G6" s="11" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>139</v>
       </c>
@@ -2119,7 +2153,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -2128,7 +2162,7 @@
       </c>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -2137,7 +2171,7 @@
       </c>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>145</v>
       </c>
@@ -2146,7 +2180,7 @@
       </c>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>147</v>
       </c>
@@ -2155,7 +2189,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>149</v>
       </c>
@@ -2166,7 +2200,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>152</v>
       </c>
@@ -2174,7 +2208,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>154</v>
       </c>
@@ -2182,7 +2216,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>156</v>
       </c>
@@ -2190,7 +2224,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>158</v>
       </c>
@@ -2198,7 +2232,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>160</v>
       </c>
@@ -2206,7 +2240,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>162</v>
       </c>
@@ -2214,7 +2248,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>164</v>
       </c>
@@ -2224,7 +2258,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>166</v>
       </c>
@@ -2242,26 +2276,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.453125"/>
+    <col min="1" max="1" width="16.42578125"/>
     <col min="2" max="2" width="39"/>
-    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="1025" width="10.7265625"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2284,7 +2318,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2304,7 +2338,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -2324,7 +2358,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -2341,7 +2375,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>173</v>
       </c>
@@ -2355,7 +2389,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>175</v>
       </c>
@@ -2366,15 +2400,18 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>177</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>179</v>
       </c>
@@ -2382,7 +2419,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>181</v>
       </c>
@@ -2390,7 +2427,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>183</v>
       </c>
@@ -2398,7 +2435,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>185</v>
       </c>
@@ -2413,26 +2450,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="1025" width="9.1796875"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2455,7 +2492,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2469,7 +2506,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -2483,7 +2520,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -2497,7 +2534,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -2511,7 +2548,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -2525,7 +2562,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>199</v>
       </c>
@@ -2539,7 +2576,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>201</v>
       </c>
@@ -2549,8 +2586,11 @@
       <c r="D8" s="7" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>203</v>
       </c>
@@ -2561,7 +2601,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>205</v>
       </c>
@@ -2572,7 +2612,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -2584,7 +2624,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>209</v>
       </c>
@@ -2595,7 +2635,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>211</v>
       </c>
@@ -2606,7 +2646,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>213</v>
       </c>
@@ -2617,7 +2657,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>215</v>
       </c>
@@ -2628,7 +2668,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>217</v>
       </c>
@@ -2639,7 +2679,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>219</v>
       </c>
@@ -2650,7 +2690,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>221</v>
       </c>
@@ -2672,25 +2712,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2713,7 +2753,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2727,7 +2767,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>223</v>
       </c>
@@ -2741,7 +2781,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>225</v>
       </c>
@@ -2755,7 +2795,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>227</v>
       </c>
@@ -2769,7 +2809,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>229</v>
       </c>
@@ -2783,7 +2823,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>231</v>
       </c>
@@ -2797,7 +2837,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>233</v>
       </c>
@@ -2811,12 +2851,15 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>235</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>236</v>
+      </c>
+      <c r="G9" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2830,22 +2873,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2868,7 +2911,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2879,7 +2922,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>237</v>
       </c>
@@ -2893,21 +2936,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2930,7 +2973,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2941,7 +2984,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -2952,4 +2995,121 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed mask with _ instead of .
</commit_message>
<xml_diff>
--- a/resources/model_variables_mask.xlsx
+++ b/resources/model_variables_mask.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvelas25\Dropbox\EAFIT-TRABAJO\Investigación\Doctorado - España\6_Proyectos\EDAR4.0\Pruebas\Model Generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvelasquez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6945" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6945" tabRatio="989" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ID_INFLUENTE" sheetId="1" r:id="rId1"/>
@@ -544,256 +544,256 @@
     <t>METEO</t>
   </si>
   <si>
+    <t>influente_MES_conc</t>
+  </si>
+  <si>
+    <t>influente_DBO5t_conc</t>
+  </si>
+  <si>
+    <t>DBO5t_1</t>
+  </si>
+  <si>
+    <t>influente_DQOt_conc</t>
+  </si>
+  <si>
+    <t>DQOt_1</t>
+  </si>
+  <si>
+    <t>influente_Pt_conc</t>
+  </si>
+  <si>
+    <t>Pt_1</t>
+  </si>
+  <si>
+    <t>influente_SO4_conc</t>
+  </si>
+  <si>
+    <t>influente_P-PO4_conc</t>
+  </si>
+  <si>
+    <t>influente_NNH4_conc</t>
+  </si>
+  <si>
+    <t>NNH4_1</t>
+  </si>
+  <si>
+    <t>influente_NTk_conc</t>
+  </si>
+  <si>
+    <t>NTk_1</t>
+  </si>
+  <si>
+    <t>CAUDAL_2</t>
+  </si>
+  <si>
+    <t>pH_1</t>
+  </si>
+  <si>
+    <t>MES_2</t>
+  </si>
+  <si>
+    <t>bios_IN_MES_conc</t>
+  </si>
+  <si>
+    <t>MESt_2</t>
+  </si>
+  <si>
+    <t>DBO5t_2</t>
+  </si>
+  <si>
+    <t>bios_IN_DBO5t_conc</t>
+  </si>
+  <si>
+    <t>DBO5t_3</t>
+  </si>
+  <si>
+    <t>bios_estado_fango_recirculacion_conc</t>
+  </si>
+  <si>
+    <t>DQOt_4</t>
+  </si>
+  <si>
+    <t>bios_IN_DQOt_conc</t>
+  </si>
+  <si>
+    <t>DQOt_5</t>
+  </si>
+  <si>
+    <t>Pt_4</t>
+  </si>
+  <si>
+    <t>bios_IN_Pt_conc</t>
+  </si>
+  <si>
+    <t>Pt_5</t>
+  </si>
+  <si>
+    <t>bios_IN_P-PO4_conc</t>
+  </si>
+  <si>
+    <t>P_PO4_1</t>
+  </si>
+  <si>
+    <t>NNH4_2</t>
+  </si>
+  <si>
+    <t>bios_IN_NNH4_conc</t>
+  </si>
+  <si>
+    <t>NNH4_3</t>
+  </si>
+  <si>
+    <t>bios_IN_NT_conc</t>
+  </si>
+  <si>
+    <t>MV_2</t>
+  </si>
+  <si>
+    <t>pH_4</t>
+  </si>
+  <si>
+    <t>MES_10</t>
+  </si>
+  <si>
+    <t>MV_1</t>
+  </si>
+  <si>
+    <t>pH_3</t>
+  </si>
+  <si>
+    <t>Cl3Fe_1</t>
+  </si>
+  <si>
+    <t>Caudal_2</t>
+  </si>
+  <si>
+    <t>Caudal_1</t>
+  </si>
+  <si>
+    <t>MES_7</t>
+  </si>
+  <si>
+    <t>Caudal_3</t>
+  </si>
+  <si>
+    <t>fangos_estado_fango_primario_a_stocker_conc</t>
+  </si>
+  <si>
+    <t>Caudal_4</t>
+  </si>
+  <si>
+    <t>MS_3</t>
+  </si>
+  <si>
+    <t>MS_7</t>
+  </si>
+  <si>
+    <t>fangos_estado_fango_biologico_a_stocker_conc</t>
+  </si>
+  <si>
+    <t>MS_9</t>
+  </si>
+  <si>
+    <t>MES_5</t>
+  </si>
+  <si>
+    <t>MV_6</t>
+  </si>
+  <si>
+    <t>MS_2</t>
+  </si>
+  <si>
+    <t>PH_2</t>
+  </si>
+  <si>
+    <t>MV_9</t>
+  </si>
+  <si>
+    <t>MS_6</t>
+  </si>
+  <si>
+    <t>PH_5</t>
+  </si>
+  <si>
+    <t>MV_10</t>
+  </si>
+  <si>
+    <t>MS_8</t>
+  </si>
+  <si>
     <t>efluente_N-NH4_conc</t>
   </si>
   <si>
     <t>efluente_N-NO3_conc</t>
   </si>
   <si>
+    <t>NTk_3</t>
+  </si>
+  <si>
     <t>efluente_Ntk_conc</t>
   </si>
   <si>
+    <t>Pt_8</t>
+  </si>
+  <si>
     <t>efluente_Pt_conc</t>
   </si>
   <si>
+    <t>P-PO4_1</t>
+  </si>
+  <si>
     <t>efluente_P-PO4_conc</t>
   </si>
   <si>
+    <t>SO4_1</t>
+  </si>
+  <si>
     <t>efluente_SO4_conc</t>
   </si>
   <si>
+    <t>DBO5t_5</t>
+  </si>
+  <si>
     <t>efluente_DBO5t_conc</t>
   </si>
   <si>
+    <t>DQOt_8</t>
+  </si>
+  <si>
     <t>efluente_DQOt_conc</t>
   </si>
   <si>
+    <t>MESt_3</t>
+  </si>
+  <si>
     <t>efluente_MES_conc</t>
   </si>
   <si>
-    <t>influente_MES_conc</t>
-  </si>
-  <si>
-    <t>influente_DBO5t_conc</t>
-  </si>
-  <si>
-    <t>influente_DQOt_conc</t>
-  </si>
-  <si>
-    <t>influente_Pt_conc</t>
-  </si>
-  <si>
-    <t>influente_SO4_conc</t>
-  </si>
-  <si>
-    <t>influente_P-PO4_conc</t>
-  </si>
-  <si>
-    <t>influente_NNH4_conc</t>
-  </si>
-  <si>
-    <t>influente_NTk_conc</t>
-  </si>
-  <si>
-    <t>bios_IN_MES_conc</t>
-  </si>
-  <si>
-    <t>bios_IN_DBO5t_conc</t>
-  </si>
-  <si>
-    <t>bios_estado_fango_recirculacion_conc</t>
-  </si>
-  <si>
-    <t>bios_IN_DQOt_conc</t>
-  </si>
-  <si>
-    <t>bios_IN_Pt_conc</t>
-  </si>
-  <si>
-    <t>bios_IN_P-PO4_conc</t>
-  </si>
-  <si>
-    <t>bios_IN_NNH4_conc</t>
-  </si>
-  <si>
-    <t>bios_IN_NT_conc</t>
-  </si>
-  <si>
-    <t>fangos_estado_fango_primario_a_stocker_conc</t>
-  </si>
-  <si>
-    <t>fangos_estado_fango_biologico_a_stocker_conc</t>
+    <t>pH_2</t>
+  </si>
+  <si>
+    <t>SST_2</t>
+  </si>
+  <si>
+    <t>DQOt_10</t>
+  </si>
+  <si>
+    <t>Pt_10</t>
+  </si>
+  <si>
+    <t>NTK_1</t>
+  </si>
+  <si>
+    <t>Caudal polimero Actiflo_ Litros /dia</t>
   </si>
   <si>
     <t>bios_IN_actiflo_MES_conc</t>
-  </si>
-  <si>
-    <t>DBO5t_1</t>
-  </si>
-  <si>
-    <t>DQOt_1</t>
-  </si>
-  <si>
-    <t>Pt_1</t>
-  </si>
-  <si>
-    <t>NNH4_1</t>
-  </si>
-  <si>
-    <t>NTk_1</t>
-  </si>
-  <si>
-    <t>CAUDAL_2</t>
-  </si>
-  <si>
-    <t>pH_1</t>
-  </si>
-  <si>
-    <t>MES_2</t>
-  </si>
-  <si>
-    <t>MESt_2</t>
-  </si>
-  <si>
-    <t>DBO5t_2</t>
-  </si>
-  <si>
-    <t>DBO5t_3</t>
-  </si>
-  <si>
-    <t>DQOt_4</t>
-  </si>
-  <si>
-    <t>DQOt_5</t>
-  </si>
-  <si>
-    <t>Pt_4</t>
-  </si>
-  <si>
-    <t>Pt_5</t>
-  </si>
-  <si>
-    <t>P_PO4_1</t>
-  </si>
-  <si>
-    <t>NNH4_2</t>
-  </si>
-  <si>
-    <t>NNH4_3</t>
-  </si>
-  <si>
-    <t>MV_2</t>
-  </si>
-  <si>
-    <t>pH_4</t>
-  </si>
-  <si>
-    <t>MES_10</t>
-  </si>
-  <si>
-    <t>MV_1</t>
-  </si>
-  <si>
-    <t>pH_3</t>
-  </si>
-  <si>
-    <t>Cl3Fe_1</t>
-  </si>
-  <si>
-    <t>Caudal_2</t>
-  </si>
-  <si>
-    <t>Caudal_1</t>
-  </si>
-  <si>
-    <t>MES_7</t>
-  </si>
-  <si>
-    <t>Caudal_3</t>
-  </si>
-  <si>
-    <t>Caudal_4</t>
-  </si>
-  <si>
-    <t>MS_3</t>
-  </si>
-  <si>
-    <t>MS_7</t>
-  </si>
-  <si>
-    <t>MS_9</t>
-  </si>
-  <si>
-    <t>MES_5</t>
-  </si>
-  <si>
-    <t>MV_6</t>
-  </si>
-  <si>
-    <t>MS_2</t>
-  </si>
-  <si>
-    <t>PH_2</t>
-  </si>
-  <si>
-    <t>MV_9</t>
-  </si>
-  <si>
-    <t>MS_6</t>
-  </si>
-  <si>
-    <t>PH_5</t>
-  </si>
-  <si>
-    <t>MV_10</t>
-  </si>
-  <si>
-    <t>MS_8</t>
-  </si>
-  <si>
-    <t>NTk_3</t>
-  </si>
-  <si>
-    <t>Pt_8</t>
-  </si>
-  <si>
-    <t>P-PO4_1</t>
-  </si>
-  <si>
-    <t>SO4_1</t>
-  </si>
-  <si>
-    <t>DBO5t_5</t>
-  </si>
-  <si>
-    <t>DQOt_8</t>
-  </si>
-  <si>
-    <t>MESt_3</t>
-  </si>
-  <si>
-    <t>pH_2</t>
-  </si>
-  <si>
-    <t>SST_2</t>
-  </si>
-  <si>
-    <t>DQOt_10</t>
-  </si>
-  <si>
-    <t>Pt_10</t>
-  </si>
-  <si>
-    <t>NTK_1</t>
-  </si>
-  <si>
-    <t>Caudal polimero Actiflo_ Litros /dia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1207,11 +1207,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
@@ -1307,7 +1307,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1315,7 +1315,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>19</v>
@@ -1340,15 +1340,15 @@
         <v>21</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>23</v>
@@ -1362,15 +1362,15 @@
         <v>23</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>25</v>
@@ -1384,18 +1384,18 @@
         <v>25</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1403,10 +1403,10 @@
         <v>27</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1414,7 +1414,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>29</v>
@@ -1428,15 +1428,15 @@
         <v>29</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>31</v>
@@ -1450,15 +1450,15 @@
         <v>31</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>7</v>
@@ -1488,7 +1488,7 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>34</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>39</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>43</v>
@@ -1600,7 +1600,7 @@
         <v>46</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>47</v>
@@ -1608,10 +1608,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>49</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>48</v>
@@ -1634,7 +1634,7 @@
         <v>51</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>52</v>
@@ -1642,13 +1642,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>53</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>53</v>
@@ -1668,7 +1668,7 @@
         <v>55</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>56</v>
@@ -1676,10 +1676,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>58</v>
@@ -1693,7 +1693,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>57</v>
@@ -1702,7 +1702,7 @@
         <v>60</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>61</v>
@@ -1710,10 +1710,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>62</v>
@@ -1730,7 +1730,7 @@
         <v>62</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>65</v>
@@ -1738,10 +1738,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>66</v>
@@ -1752,13 +1752,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>66</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>68</v>
@@ -1766,10 +1766,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>69</v>
@@ -1783,7 +1783,7 @@
         <v>69</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1791,7 +1791,7 @@
         <v>71</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1804,7 +1804,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>40</v>
@@ -1836,7 +1836,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>51</v>
@@ -1844,15 +1844,15 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>55</v>
@@ -1860,7 +1860,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>58</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>41</v>
@@ -1892,7 +1892,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>45</v>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>67</v>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>68</v>
@@ -2000,7 +2000,7 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>87</v>
@@ -2067,7 +2067,7 @@
         <v>94</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>89</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>89</v>
@@ -2098,7 +2098,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>90</v>
@@ -2118,7 +2118,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>91</v>
@@ -2127,7 +2127,7 @@
         <v>105</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>99</v>
@@ -2155,7 +2155,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>94</v>
@@ -2182,7 +2182,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>99</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>100</v>
@@ -2202,15 +2202,15 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>102</v>
@@ -2218,7 +2218,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>103</v>
@@ -2226,15 +2226,15 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>104</v>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>105</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>106</v>
@@ -2283,7 +2283,7 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125"/>
     <col min="2" max="2" width="39"/>
@@ -2454,10 +2454,10 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
@@ -2511,10 +2511,10 @@
         <v>130</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>169</v>
+        <v>228</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>169</v>
+        <v>228</v>
       </c>
       <c r="G3" t="s">
         <v>131</v>
@@ -2525,10 +2525,10 @@
         <v>132</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>170</v>
+        <v>229</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>170</v>
+        <v>229</v>
       </c>
       <c r="G4" t="s">
         <v>133</v>
@@ -2536,13 +2536,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>171</v>
+        <v>231</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>171</v>
+        <v>231</v>
       </c>
       <c r="G5" t="s">
         <v>37</v>
@@ -2550,13 +2550,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>172</v>
+        <v>233</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>172</v>
+        <v>233</v>
       </c>
       <c r="G6" t="s">
         <v>160</v>
@@ -2564,13 +2564,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>173</v>
+        <v>235</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>173</v>
+        <v>235</v>
       </c>
       <c r="G7" t="s">
         <v>161</v>
@@ -2578,13 +2578,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>174</v>
+        <v>237</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>174</v>
+        <v>237</v>
       </c>
       <c r="G8" t="s">
         <v>168</v>
@@ -2592,36 +2592,36 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>175</v>
+        <v>239</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>175</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>176</v>
+        <v>241</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>176</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>177</v>
+        <v>243</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="7" t="s">
-        <v>177</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2637,7 +2637,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>136</v>
@@ -2648,7 +2648,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>137</v>
@@ -2670,7 +2670,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>140</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>141</v>
@@ -2692,7 +2692,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>142</v>
@@ -2719,7 +2719,7 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
@@ -2877,10 +2877,10 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
@@ -2924,7 +2924,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>157</v>
@@ -2939,11 +2939,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
@@ -2981,15 +2981,15 @@
         <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>196</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>196</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3005,7 +3005,7 @@
       <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">

</xml_diff>

<commit_message>
Added ID_ELECTRICIDAD to vars mask
</commit_message>
<xml_diff>
--- a/resources/model_variables_mask.xlsx
+++ b/resources/model_variables_mask.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvelasquez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvelas25\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6945" tabRatio="989" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6945" tabRatio="989" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ID_INFLUENTE" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="252">
   <si>
     <t>ORIGEN</t>
   </si>
@@ -788,13 +788,16 @@
   </si>
   <si>
     <t>bios_IN_actiflo_MES_conc</t>
+  </si>
+  <si>
+    <t>ID_ELECTRICIDAD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -820,6 +823,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -872,7 +883,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -891,6 +902,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1211,7 +1223,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
@@ -1488,7 +1500,7 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
@@ -2000,7 +2012,7 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
@@ -2283,7 +2295,7 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125"/>
     <col min="2" max="2" width="39"/>
@@ -2453,11 +2465,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
@@ -2600,6 +2612,9 @@
       <c r="D9" s="14" t="s">
         <v>239</v>
       </c>
+      <c r="G9" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2611,6 +2626,7 @@
       <c r="D10" s="7" t="s">
         <v>241</v>
       </c>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2703,7 +2719,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2716,10 +2732,10 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
@@ -2880,7 +2896,7 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
@@ -2939,11 +2955,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
@@ -3005,7 +3021,7 @@
       <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">

</xml_diff>